<commit_message>
ADIT: finalizado disc. artigo, inicio analise multivariada
</commit_message>
<xml_diff>
--- a/imagens/notebooks/dados experimentais/propriedades_aditivos.xlsx
+++ b/imagens/notebooks/dados experimentais/propriedades_aditivos.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Doutorado\Tese\imagens\notebooks\dados experimentais\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82063D21-A28A-4B10-A55B-48D6D5DC45D3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8871ADB-CE5E-4E04-A56E-9E592E9953E1}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{57FECDDB-C691-4F58-BAFA-D5EE86D39B17}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="3" xr2:uid="{57FECDDB-C691-4F58-BAFA-D5EE86D39B17}"/>
   </bookViews>
   <sheets>
     <sheet name="n" sheetId="1" r:id="rId1"/>
     <sheet name="eps" sheetId="2" r:id="rId2"/>
+    <sheet name="G" sheetId="3" r:id="rId3"/>
+    <sheet name="Tens" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="16">
   <si>
     <t>Água</t>
   </si>
@@ -63,6 +65,18 @@
   <si>
     <t>Agua</t>
   </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>err</t>
+  </si>
+  <si>
+    <t>TS</t>
+  </si>
+  <si>
+    <t>Err</t>
+  </si>
 </sst>
 </file>
 
@@ -97,8 +111,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1456,7 +1474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{121F8C99-396E-4761-B448-084FEBB96625}">
   <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
@@ -1899,4 +1917,869 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C617A72E-DD73-46F0-AF6D-3E97C8B63C47}">
+  <dimension ref="A1:R12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>12</v>
+      </c>
+      <c r="R2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f>A1&amp;" "&amp;A2</f>
+        <v>Ureia p</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:C3" si="0">B1&amp;" "&amp;B2</f>
+        <v>Ureia G</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v>Ureia err</v>
+      </c>
+      <c r="D3" t="str">
+        <f>D1&amp;" "&amp;D2</f>
+        <v>Glicerol p</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3" si="1">E1&amp;" "&amp;E2</f>
+        <v>Glicerol G</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3" si="2">F1&amp;" "&amp;F2</f>
+        <v>Glicerol err</v>
+      </c>
+      <c r="G3" t="str">
+        <f>G1&amp;" "&amp;G2</f>
+        <v>Sacarose p</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3" si="3">H1&amp;" "&amp;H2</f>
+        <v>Sacarose G</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3" si="4">I1&amp;" "&amp;I2</f>
+        <v>Sacarose err</v>
+      </c>
+      <c r="J3" t="str">
+        <f>J1&amp;" "&amp;J2</f>
+        <v>DMSO p</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" ref="K3" si="5">K1&amp;" "&amp;K2</f>
+        <v>DMSO G</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" ref="L3" si="6">L1&amp;" "&amp;L2</f>
+        <v>DMSO err</v>
+      </c>
+      <c r="M3" t="str">
+        <f>M1&amp;" "&amp;M2</f>
+        <v>13BD p</v>
+      </c>
+      <c r="N3" t="str">
+        <f t="shared" ref="N3" si="7">N1&amp;" "&amp;N2</f>
+        <v>13BD G</v>
+      </c>
+      <c r="O3" t="str">
+        <f t="shared" ref="O3" si="8">O1&amp;" "&amp;O2</f>
+        <v>13BD err</v>
+      </c>
+      <c r="P3" t="str">
+        <f>P1&amp;" "&amp;P2</f>
+        <v>Água p</v>
+      </c>
+      <c r="Q3" t="str">
+        <f t="shared" ref="Q3" si="9">Q1&amp;" "&amp;Q2</f>
+        <v>Água G</v>
+      </c>
+      <c r="R3" t="str">
+        <f t="shared" ref="R3" si="10">R1&amp;" "&amp;R2</f>
+        <v>Água err</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>2.7273076669559635</v>
+      </c>
+      <c r="C4">
+        <v>1.0591568922954818E-2</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>2.7495960843032785</v>
+      </c>
+      <c r="F4">
+        <v>1.0755380976490425E-2</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <v>2.7687733460708999</v>
+      </c>
+      <c r="I4">
+        <v>1.1872647108468731E-2</v>
+      </c>
+      <c r="J4">
+        <v>5</v>
+      </c>
+      <c r="K4">
+        <v>2.639503963422122</v>
+      </c>
+      <c r="L4">
+        <v>1.0915838946093874E-2</v>
+      </c>
+      <c r="M4">
+        <v>5</v>
+      </c>
+      <c r="N4">
+        <v>2.44282633634029</v>
+      </c>
+      <c r="O4">
+        <v>1.6039468039188407E-2</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>2.7769885124686891</v>
+      </c>
+      <c r="R4">
+        <v>1.5655740151519902E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>2.7004459239408591</v>
+      </c>
+      <c r="C5">
+        <v>6.0731489463343351E-3</v>
+      </c>
+      <c r="D5">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>2.6500844816133431</v>
+      </c>
+      <c r="F5">
+        <v>7.1135760897916402E-3</v>
+      </c>
+      <c r="G5">
+        <v>15</v>
+      </c>
+      <c r="H5">
+        <v>2.746373017787358</v>
+      </c>
+      <c r="I5">
+        <v>1.0807828310454617E-2</v>
+      </c>
+      <c r="J5">
+        <v>15</v>
+      </c>
+      <c r="K5">
+        <v>2.4433520677507552</v>
+      </c>
+      <c r="L5">
+        <v>4.0469904103252654E-3</v>
+      </c>
+      <c r="M5">
+        <v>15</v>
+      </c>
+      <c r="N5">
+        <v>2.1086807489690607</v>
+      </c>
+      <c r="O5">
+        <v>3.3227681695107234E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>25</v>
+      </c>
+      <c r="B6">
+        <v>2.6242753459435471</v>
+      </c>
+      <c r="C6">
+        <v>2.9597143266045307E-2</v>
+      </c>
+      <c r="D6">
+        <v>25</v>
+      </c>
+      <c r="E6">
+        <v>2.567377335160133</v>
+      </c>
+      <c r="F6">
+        <v>9.5904734096390505E-3</v>
+      </c>
+      <c r="G6">
+        <v>25</v>
+      </c>
+      <c r="H6">
+        <v>2.7774094375416238</v>
+      </c>
+      <c r="I6">
+        <v>7.3741062344460174E-3</v>
+      </c>
+      <c r="J6">
+        <v>25</v>
+      </c>
+      <c r="K6">
+        <v>2.2934656146895489</v>
+      </c>
+      <c r="L6">
+        <v>4.4896141206617127E-3</v>
+      </c>
+      <c r="M6">
+        <v>25</v>
+      </c>
+      <c r="N6">
+        <v>1.8989904622544598</v>
+      </c>
+      <c r="O6">
+        <v>3.4206354419220471E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>35</v>
+      </c>
+      <c r="B7">
+        <v>2.6531795840526047</v>
+      </c>
+      <c r="C7">
+        <v>1.4397899149253397E-2</v>
+      </c>
+      <c r="D7">
+        <v>35</v>
+      </c>
+      <c r="E7">
+        <v>2.4089232574810708</v>
+      </c>
+      <c r="F7">
+        <v>3.1748067354976435E-2</v>
+      </c>
+      <c r="G7">
+        <v>35</v>
+      </c>
+      <c r="H7">
+        <v>2.7687571987213189</v>
+      </c>
+      <c r="I7">
+        <v>2.4849962486751982E-2</v>
+      </c>
+      <c r="J7">
+        <v>35</v>
+      </c>
+      <c r="K7">
+        <v>2.1560708301387952</v>
+      </c>
+      <c r="L7">
+        <v>5.4718202935239105E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>45</v>
+      </c>
+      <c r="E8">
+        <v>2.3591283987202516</v>
+      </c>
+      <c r="F8">
+        <v>5.539231864917683E-3</v>
+      </c>
+      <c r="G8">
+        <v>45</v>
+      </c>
+      <c r="H8">
+        <v>2.7683968450157979</v>
+      </c>
+      <c r="I8">
+        <v>8.2823632389656329E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>65</v>
+      </c>
+      <c r="E9">
+        <v>2.177661603512711</v>
+      </c>
+      <c r="F9">
+        <v>5.6755534297880331E-3</v>
+      </c>
+      <c r="G9">
+        <v>65</v>
+      </c>
+      <c r="H9">
+        <v>2.7705484756649676</v>
+      </c>
+      <c r="I9">
+        <v>1.6701557828426646E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F371A25C-61FE-4198-96D3-DEFB541AF18F}">
+  <dimension ref="A1:R9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f>A1&amp;" "&amp;A2</f>
+        <v>Ureia p</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:C3" si="0">B1&amp;" "&amp;B2</f>
+        <v>Ureia TS</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v>Ureia Err</v>
+      </c>
+      <c r="D3" t="str">
+        <f>D1&amp;" "&amp;D2</f>
+        <v>Glicerol p</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:F3" si="1">E1&amp;" "&amp;E2</f>
+        <v>Glicerol TS</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" si="1"/>
+        <v>Glicerol Err</v>
+      </c>
+      <c r="G3" t="str">
+        <f>G1&amp;" "&amp;G2</f>
+        <v>Sacarose p</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" ref="H3:I3" si="2">H1&amp;" "&amp;H2</f>
+        <v>Sacarose TS</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" si="2"/>
+        <v>Sacarose Err</v>
+      </c>
+      <c r="J3" t="str">
+        <f>J1&amp;" "&amp;J2</f>
+        <v>DMSO p</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:L3" si="3">K1&amp;" "&amp;K2</f>
+        <v>DMSO TS</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" si="3"/>
+        <v>DMSO Err</v>
+      </c>
+      <c r="M3" t="str">
+        <f>M1&amp;" "&amp;M2</f>
+        <v>13BD p</v>
+      </c>
+      <c r="N3" t="str">
+        <f t="shared" ref="N3:O3" si="4">N1&amp;" "&amp;N2</f>
+        <v>13BD TS</v>
+      </c>
+      <c r="O3" t="str">
+        <f t="shared" si="4"/>
+        <v>13BD Err</v>
+      </c>
+      <c r="P3" t="str">
+        <f>P1&amp;" "&amp;P2</f>
+        <v>Água p</v>
+      </c>
+      <c r="Q3" t="str">
+        <f t="shared" ref="Q3:R3" si="5">Q1&amp;" "&amp;Q2</f>
+        <v>Água TS</v>
+      </c>
+      <c r="R3" t="str">
+        <f t="shared" si="5"/>
+        <v>Água Err</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>72.105631931978394</v>
+      </c>
+      <c r="C4">
+        <v>0.28002406167587407</v>
+      </c>
+      <c r="D4" s="2">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>72.860451678802477</v>
+      </c>
+      <c r="F4">
+        <v>0.28500255742954311</v>
+      </c>
+      <c r="G4" s="2">
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <v>72.832528072504346</v>
+      </c>
+      <c r="I4">
+        <v>0.31230974722058152</v>
+      </c>
+      <c r="J4" s="2">
+        <v>5</v>
+      </c>
+      <c r="K4">
+        <v>70.115287670817906</v>
+      </c>
+      <c r="L4">
+        <v>0.28996629612231756</v>
+      </c>
+      <c r="M4" s="2">
+        <v>5</v>
+      </c>
+      <c r="N4">
+        <v>64.722802694327925</v>
+      </c>
+      <c r="O4">
+        <v>0.42496648647468899</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>72.841853234209069</v>
+      </c>
+      <c r="R4">
+        <v>0.41065820808028453</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>72.58773559212122</v>
+      </c>
+      <c r="C5">
+        <v>0.16324567954493907</v>
+      </c>
+      <c r="D5" s="2">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>71.818146593770763</v>
+      </c>
+      <c r="F5">
+        <v>0.19278021284497995</v>
+      </c>
+      <c r="G5" s="2">
+        <v>15</v>
+      </c>
+      <c r="H5">
+        <v>72.708269723579647</v>
+      </c>
+      <c r="I5">
+        <v>0.2861295573591735</v>
+      </c>
+      <c r="J5" s="2">
+        <v>15</v>
+      </c>
+      <c r="K5">
+        <v>66.605784155999089</v>
+      </c>
+      <c r="L5">
+        <v>0.11032096983045986</v>
+      </c>
+      <c r="M5" s="2">
+        <v>15</v>
+      </c>
+      <c r="N5">
+        <v>57.17538780870791</v>
+      </c>
+      <c r="O5">
+        <v>9.0094509936171269E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>25</v>
+      </c>
+      <c r="B6">
+        <v>71.862282272757213</v>
+      </c>
+      <c r="C6">
+        <v>0.81047831628622757</v>
+      </c>
+      <c r="D6" s="2">
+        <v>25</v>
+      </c>
+      <c r="E6">
+        <v>71.291805894042781</v>
+      </c>
+      <c r="F6">
+        <v>0.26631152319856427</v>
+      </c>
+      <c r="G6" s="2">
+        <v>25</v>
+      </c>
+      <c r="H6">
+        <v>74.122389236354678</v>
+      </c>
+      <c r="I6">
+        <v>0.19679718992516956</v>
+      </c>
+      <c r="J6" s="2">
+        <v>25</v>
+      </c>
+      <c r="K6">
+        <v>64.272945899777525</v>
+      </c>
+      <c r="L6">
+        <v>0.12581864041908825</v>
+      </c>
+      <c r="M6" s="2">
+        <v>25</v>
+      </c>
+      <c r="N6">
+        <v>52.76782548511602</v>
+      </c>
+      <c r="O6">
+        <v>9.5050237289374465E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>35</v>
+      </c>
+      <c r="B7">
+        <v>74.197394116130795</v>
+      </c>
+      <c r="C7">
+        <v>0.40264390847968989</v>
+      </c>
+      <c r="D7" s="2">
+        <v>35</v>
+      </c>
+      <c r="E7">
+        <v>68.230956628253693</v>
+      </c>
+      <c r="F7">
+        <v>0.98497375901154538</v>
+      </c>
+      <c r="G7" s="2">
+        <v>35</v>
+      </c>
+      <c r="H7">
+        <v>74.628050894832128</v>
+      </c>
+      <c r="I7">
+        <v>0.66979663874190642</v>
+      </c>
+      <c r="J7" s="2">
+        <v>35</v>
+      </c>
+      <c r="K7">
+        <v>62.281004200190289</v>
+      </c>
+      <c r="L7">
+        <v>0.1580608846054056</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D8" s="2">
+        <v>45</v>
+      </c>
+      <c r="E8">
+        <v>69.592757647526582</v>
+      </c>
+      <c r="F8">
+        <v>0.16340374730675472</v>
+      </c>
+      <c r="G8" s="2">
+        <v>45</v>
+      </c>
+      <c r="H8">
+        <v>75.555133412247116</v>
+      </c>
+      <c r="I8">
+        <v>0.22604239728685593</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D9" s="2">
+        <v>65</v>
+      </c>
+      <c r="E9">
+        <v>68.97442559653804</v>
+      </c>
+      <c r="F9">
+        <v>0.17976532126507963</v>
+      </c>
+      <c r="G9" s="2">
+        <v>65</v>
+      </c>
+      <c r="H9">
+        <v>78.65753344371349</v>
+      </c>
+      <c r="I9">
+        <v>0.47416724702363416</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>